<commit_message>
added annotations work in prograess
</commit_message>
<xml_diff>
--- a/data/external/posts_to_annotate.xlsx
+++ b/data/external/posts_to_annotate.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbu\Desktop\Bachelor_Thesis\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0629DE1B-AB88-4E8B-AC87-1967EF175669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF704690-389D-4ECA-B8BA-95CB71E5F832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{448BB4A0-4DD9-49CB-8D80-C9D34A186E58}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{448BB4A0-4DD9-49CB-8D80-C9D34A186E58}"/>
   </bookViews>
   <sheets>
-    <sheet name="data-1654883132672" sheetId="2" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="data" sheetId="2" r:id="rId1"/>
+    <sheet name="wsb_expressions" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">'data-1654883132672'!$A$1:$C$2001</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">data!$A$1:$C$2001</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4003" uniqueCount="2499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4025" uniqueCount="2521">
   <si>
     <t>id</t>
   </si>
@@ -8718,18 +8719,90 @@
   <si>
     <t>does not take much SKLZ to lose money.</t>
   </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>sell</t>
+  </si>
+  <si>
+    <t>bullish</t>
+  </si>
+  <si>
+    <t>bearish</t>
+  </si>
+  <si>
+    <t>Apes Together Strong</t>
+  </si>
+  <si>
+    <t>Paper Hands</t>
+  </si>
+  <si>
+    <t>TDM</t>
+  </si>
+  <si>
+    <t>moon</t>
+  </si>
+  <si>
+    <t>btfd</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>buy the fucking dip</t>
+  </si>
+  <si>
+    <t>double down</t>
+  </si>
+  <si>
+    <t>hold</t>
+  </si>
+  <si>
+    <t>pump and dump</t>
+  </si>
+  <si>
+    <t>rocket ship</t>
+  </si>
+  <si>
+    <t>andromeda</t>
+  </si>
+  <si>
+    <t>diamond hands</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -8752,12 +8825,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -8781,30 +8855,32 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" connectionId="1" xr16:uid="{57B82794-2E6F-4E0B-82CC-99341ABB7ED5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="4">
-    <queryTableFields count="3">
+  <queryTableRefresh nextId="6" unboundColumnsRight="1">
+    <queryTableFields count="4">
       <queryTableField id="1" name="id" tableColumnId="1"/>
       <queryTableField id="2" name="post" tableColumnId="2"/>
       <queryTableField id="3" name="stock_symbol" tableColumnId="3"/>
+      <queryTableField id="4" dataBound="0" tableColumnId="4"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BFF5C33-6C01-4423-B39E-55A6663C6FDA}" name="data_1654883132672" displayName="data_1654883132672" ref="A1:C2001" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C2001" xr:uid="{1BFF5C33-6C01-4423-B39E-55A6663C6FDA}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BFF5C33-6C01-4423-B39E-55A6663C6FDA}" name="data_1654883132672" displayName="data_1654883132672" ref="A1:D2001" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D2001" xr:uid="{1BFF5C33-6C01-4423-B39E-55A6663C6FDA}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D81734F3-F66C-4974-B6DC-CD3DBAD7E35F}" uniqueName="1" name="id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{33C1FB28-2E52-46EE-B74D-EE7F31678C4C}" uniqueName="2" name="post" queryTableFieldId="2" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{36B9606C-9450-4A72-B59F-E47E51E9A140}" uniqueName="3" name="stock_symbol" queryTableFieldId="3" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{35328C3A-859C-4423-8AFB-AA4491CD225E}" uniqueName="4" name="Annotation" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9100,20 +9176,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D95F4C-0BA2-4529-863C-83ADFFF0672B}">
-  <dimension ref="A1:C2001"/>
+  <dimension ref="A1:D2001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9123,8 +9200,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9438588</v>
       </c>
@@ -9135,7 +9215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3153666</v>
       </c>
@@ -9145,8 +9225,11 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12497670</v>
       </c>
@@ -9156,8 +9239,11 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2885708</v>
       </c>
@@ -9167,8 +9253,11 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9477011</v>
       </c>
@@ -9179,7 +9268,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12766073</v>
       </c>
@@ -9190,7 +9279,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7776910</v>
       </c>
@@ -9200,8 +9289,11 @@
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3375035</v>
       </c>
@@ -9211,8 +9303,11 @@
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3264567</v>
       </c>
@@ -9223,7 +9318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10551344</v>
       </c>
@@ -9234,7 +9329,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11008902</v>
       </c>
@@ -9244,8 +9339,11 @@
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1252991</v>
       </c>
@@ -9255,8 +9353,11 @@
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2136489</v>
       </c>
@@ -9266,8 +9367,11 @@
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10271388</v>
       </c>
@@ -9277,8 +9381,11 @@
       <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1939122</v>
       </c>
@@ -9288,8 +9395,11 @@
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13089093</v>
       </c>
@@ -9299,8 +9409,11 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8087282</v>
       </c>
@@ -9311,7 +9424,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13746836</v>
       </c>
@@ -9322,7 +9435,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13352969</v>
       </c>
@@ -9333,7 +9446,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12643966</v>
       </c>
@@ -9343,8 +9456,11 @@
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9893769</v>
       </c>
@@ -9355,7 +9471,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7116686</v>
       </c>
@@ -9365,8 +9481,11 @@
       <c r="C23" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1395579</v>
       </c>
@@ -9377,7 +9496,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2832086</v>
       </c>
@@ -9387,8 +9506,11 @@
       <c r="C25" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1188267</v>
       </c>
@@ -9398,8 +9520,11 @@
       <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9073895</v>
       </c>
@@ -9409,8 +9534,11 @@
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9378643</v>
       </c>
@@ -9420,8 +9548,11 @@
       <c r="C28" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1869978</v>
       </c>
@@ -9432,7 +9563,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5159312</v>
       </c>
@@ -9442,8 +9573,11 @@
       <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5926652</v>
       </c>
@@ -9454,7 +9588,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>14384717</v>
       </c>
@@ -9464,8 +9598,11 @@
       <c r="C32" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10305083</v>
       </c>
@@ -9475,8 +9612,11 @@
       <c r="C33" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>14320817</v>
       </c>
@@ -9486,8 +9626,11 @@
       <c r="C34" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1945048</v>
       </c>
@@ -9498,7 +9641,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>202052</v>
       </c>
@@ -9508,8 +9651,11 @@
       <c r="C36" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>14415201</v>
       </c>
@@ -9519,8 +9665,11 @@
       <c r="C37" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>14364022</v>
       </c>
@@ -9530,8 +9679,11 @@
       <c r="C38" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1940063</v>
       </c>
@@ -9541,8 +9693,11 @@
       <c r="C39" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>14633708</v>
       </c>
@@ -9553,7 +9708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1104390</v>
       </c>
@@ -9564,7 +9719,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>12934410</v>
       </c>
@@ -9575,7 +9730,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>14334345</v>
       </c>
@@ -9585,8 +9740,11 @@
       <c r="C43" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>11923423</v>
       </c>
@@ -9596,8 +9754,11 @@
       <c r="C44" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>11455978</v>
       </c>
@@ -9607,8 +9768,11 @@
       <c r="C45" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4351082</v>
       </c>
@@ -9618,8 +9782,11 @@
       <c r="C46" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5201633</v>
       </c>
@@ -9629,8 +9796,11 @@
       <c r="C47" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>4143290</v>
       </c>
@@ -9641,7 +9811,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>8925577</v>
       </c>
@@ -9651,8 +9821,11 @@
       <c r="C49" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1948818</v>
       </c>
@@ -9662,8 +9835,11 @@
       <c r="C50" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>13365525</v>
       </c>
@@ -9674,7 +9850,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2674726</v>
       </c>
@@ -9685,7 +9861,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4612898</v>
       </c>
@@ -9696,7 +9872,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7180838</v>
       </c>
@@ -9707,7 +9883,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4489156</v>
       </c>
@@ -9718,7 +9894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7519409</v>
       </c>
@@ -9729,7 +9905,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1090265</v>
       </c>
@@ -9739,8 +9915,11 @@
       <c r="C57" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>13308766</v>
       </c>
@@ -9751,7 +9930,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9356224</v>
       </c>
@@ -9762,7 +9941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>12661174</v>
       </c>
@@ -9773,7 +9952,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>13829963</v>
       </c>
@@ -9783,8 +9962,11 @@
       <c r="C61" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5615618</v>
       </c>
@@ -9795,7 +9977,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3189296</v>
       </c>
@@ -9806,7 +9988,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>8711125</v>
       </c>
@@ -9817,7 +9999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>12571293</v>
       </c>
@@ -9827,8 +10009,11 @@
       <c r="C65" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5254915</v>
       </c>
@@ -9839,7 +10024,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3551659</v>
       </c>
@@ -9850,7 +10035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>14377157</v>
       </c>
@@ -9861,7 +10046,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>11768533</v>
       </c>
@@ -9872,7 +10057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>10060611</v>
       </c>
@@ -9883,7 +10068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3148322</v>
       </c>
@@ -9894,7 +10079,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9640425</v>
       </c>
@@ -9905,7 +10090,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2188476</v>
       </c>
@@ -9916,7 +10101,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1306559</v>
       </c>
@@ -9927,7 +10112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>13077034</v>
       </c>
@@ -9938,7 +10123,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>3496865</v>
       </c>
@@ -9949,7 +10134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>14362994</v>
       </c>
@@ -9960,7 +10145,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>8372010</v>
       </c>
@@ -9971,7 +10156,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>8562366</v>
       </c>
@@ -9982,7 +10167,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2224283</v>
       </c>
@@ -31113,7 +31298,7 @@
         <v>2497</v>
       </c>
     </row>
-    <row r="2001" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2001" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2001">
         <v>6686266</v>
       </c>
@@ -31122,6 +31307,9 @@
       </c>
       <c r="C2001" s="1" t="s">
         <v>1628</v>
+      </c>
+      <c r="D2001">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -31134,13 +31322,179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F26F3A4-A931-436E-833B-F44C2FA4E370}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2500</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2501</v>
+      </c>
+      <c r="E1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2502</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2503</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2504</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2505</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2506</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2507</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2512</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2509</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2520</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2510</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2513</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2517</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2508</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2511</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2514</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2515</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2518</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2519</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F22" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>